<commit_message>
Updated employee login details to include employee ids
</commit_message>
<xml_diff>
--- a/Database/Employee Login details.xlsx
+++ b/Database/Employee Login details.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="84">
   <si>
     <t>John</t>
   </si>
@@ -207,6 +207,75 @@
   </si>
   <si>
     <t>driver</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>testpassword123</t>
+  </si>
+  <si>
+    <t>A1019</t>
+  </si>
+  <si>
+    <t>D1006</t>
+  </si>
+  <si>
+    <t>D1020</t>
+  </si>
+  <si>
+    <t>D1021</t>
+  </si>
+  <si>
+    <t>D1022</t>
+  </si>
+  <si>
+    <t>D1023</t>
+  </si>
+  <si>
+    <t>D1024</t>
+  </si>
+  <si>
+    <t>D1025</t>
+  </si>
+  <si>
+    <t>D1026</t>
+  </si>
+  <si>
+    <t>D1027</t>
+  </si>
+  <si>
+    <t>A1028</t>
+  </si>
+  <si>
+    <t>D1029</t>
+  </si>
+  <si>
+    <t>D1030</t>
+  </si>
+  <si>
+    <t>D1031</t>
+  </si>
+  <si>
+    <t>D1032</t>
+  </si>
+  <si>
+    <t>A1033</t>
+  </si>
+  <si>
+    <t>A1034</t>
+  </si>
+  <si>
+    <t>A1035</t>
+  </si>
+  <si>
+    <t>D1036</t>
+  </si>
+  <si>
+    <t>D1037</t>
+  </si>
+  <si>
+    <t>D1038</t>
   </si>
 </sst>
 </file>
@@ -524,295 +593,373 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
         <v>40</v>
       </c>
-      <c r="D2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
         <v>41</v>
       </c>
-      <c r="D3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
         <v>42</v>
       </c>
-      <c r="D4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="E5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
         <v>34</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>35</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D6" t="s">
         <v>43</v>
       </c>
-      <c r="D5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D7" t="s">
         <v>44</v>
       </c>
-      <c r="D6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D8" t="s">
         <v>45</v>
       </c>
-      <c r="D7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D9" t="s">
         <v>46</v>
       </c>
-      <c r="D8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="E9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D10" t="s">
         <v>47</v>
       </c>
-      <c r="D9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="E10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C11" t="s">
         <v>17</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D11" t="s">
         <v>48</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" t="s">
         <v>37</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C12" t="s">
         <v>36</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D12" t="s">
         <v>49</v>
       </c>
-      <c r="D11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="E12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" t="s">
         <v>18</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C13" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D13" t="s">
         <v>50</v>
       </c>
-      <c r="D12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="E13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C14" t="s">
         <v>21</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D14" t="s">
         <v>51</v>
       </c>
-      <c r="D13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="E14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" t="s">
         <v>22</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C15" t="s">
         <v>23</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D15" t="s">
         <v>52</v>
       </c>
-      <c r="D14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="E15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" t="s">
         <v>24</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C16" t="s">
         <v>25</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D16" t="s">
         <v>53</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" t="s">
         <v>26</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C17" t="s">
         <v>27</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D17" t="s">
         <v>54</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E17" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" t="s">
         <v>28</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C18" t="s">
         <v>29</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D18" t="s">
         <v>55</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" t="s">
         <v>30</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C19" t="s">
         <v>31</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D19" t="s">
         <v>56</v>
       </c>
-      <c r="D18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="E19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" t="s">
         <v>32</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C20" t="s">
         <v>33</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D20" t="s">
         <v>57</v>
       </c>
-      <c r="D19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="E20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" t="s">
         <v>38</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C21" t="s">
         <v>39</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D21" t="s">
         <v>58</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E21" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>